<commit_message>
add dynamic plot method in serial port
</commit_message>
<xml_diff>
--- a/example/motor_data/customsig.xlsx
+++ b/example/motor_data/customsig.xlsx
@@ -348,10 +348,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A323"/>
+  <dimension ref="A1:A625"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K323" sqref="K323"/>
+    <sheetView tabSelected="1" topLeftCell="A609" workbookViewId="0">
+      <selection activeCell="G617" sqref="G617"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1971,6 +1971,1516 @@
         <v>5</v>
       </c>
     </row>
+    <row r="324" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A324">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="325" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A325">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="326" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A326">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="327" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A327">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="328" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A328">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="329" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A329">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="330" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A330">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="331" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A331">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="332" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A332">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="333" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A333">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="334" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A334">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="335" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A335">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="336" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A336">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="337" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A337">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="338" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A338">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="339" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A339">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="340" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A340">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="341" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A341">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="342" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A342">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="343" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A343">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="344" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A344">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="345" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A345">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="346" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A346">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="347" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A347">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="348" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A348">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="349" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A349">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="350" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A350">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="351" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A351">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="352" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A352">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="353" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A353">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="354" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A354">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="355" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A355">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="356" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A356">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="357" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A357">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="358" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A358">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="359" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A359">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="360" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A360">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="361" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A361">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="362" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A362">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="363" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A363">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="364" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A364">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="365" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A365">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A366">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A367">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A368">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="369" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A369">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A370">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A371">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A372">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A373">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="374" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A374">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="375" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A375">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="376" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A376">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="377" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A377">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="378" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A378">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="379" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A379">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="380" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A380">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="381" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A381">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="382" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A382">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="383" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A383">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="384" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A384">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="385" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A385">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="386" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A386">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="387" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A387">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="388" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A388">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="389" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A389">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="390" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A390">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="391" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A391">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="392" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A392">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="393" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A393">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="394" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A394">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="395" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A395">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="396" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A396">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="397" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A397">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="398" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A398">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="399" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A399">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="400" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A400">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="401" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A401">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="402" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A402">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="403" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A403">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="404" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A404">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="405" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A405">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="406" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A406">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="407" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A407">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="408" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A408">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="409" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A409">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="410" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A410">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="411" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A411">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="412" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A412">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="413" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A413">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="414" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A414">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="415" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A415">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="416" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A416">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="417" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A417">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="418" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A418">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="419" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A419">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="420" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A420">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="421" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A421">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="422" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A422">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="423" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A423">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="424" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A424">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="425" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A425">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="426" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A426">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="427" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A427">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="428" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A428">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="429" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A429">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="430" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A430">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="431" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A431">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="432" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A432">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="433" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A433">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="434" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A434">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="435" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A435">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="436" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A436">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="437" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A437">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="438" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A438">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="439" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A439">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="440" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A440">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="441" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A441">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="442" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A442">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="443" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A443">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="444" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A444">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="445" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A445">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="446" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A446">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="447" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A447">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="448" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A448">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="449" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A449">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="450" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A450">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="451" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A451">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="452" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A452">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="453" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A453">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="454" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A454">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="455" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A455">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="456" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A456">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="457" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A457">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="458" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A458">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="459" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A459">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="460" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A460">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="461" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A461">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="462" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A462">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="463" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A463">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="464" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A464">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="465" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A465">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="466" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A466">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="467" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A467">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="468" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A468">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="469" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A469">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="470" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A470">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="471" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A471">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="472" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A472">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="473" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A473">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="474" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A474">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="475" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A475">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="476" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A476">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="477" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A477">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="478" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A478">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="479" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A479">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="480" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A480">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="481" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A481">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="482" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A482">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="483" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A483">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="484" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A484">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="485" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A485">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="486" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A486">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="487" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A487">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="488" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A488">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="489" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A489">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="490" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A490">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="491" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A491">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="492" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A492">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="493" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A493">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="494" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A494">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="495" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A495">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="496" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A496">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="497" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A497">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="498" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A498">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="499" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A499">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="500" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A500">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="501" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A501">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="502" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A502">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="503" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A503">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="504" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A504">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="505" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A505">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="506" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A506">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="507" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A507">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="508" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A508">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="509" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A509">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="510" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A510">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="511" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A511">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="512" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A512">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="513" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A513">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="514" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A514">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="515" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A515">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="516" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A516">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="517" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A517">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="518" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A518">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="519" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A519">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="520" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A520">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="521" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A521">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="522" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A522">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="523" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A523">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="524" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A524">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="525" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A525">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="526" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A526">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="527" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A527">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="528" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A528">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="529" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A529">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="530" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A530">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="531" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A531">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="532" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A532">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="533" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A533">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="534" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A534">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="535" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A535">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="536" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A536">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="537" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A537">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="538" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A538">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="539" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A539">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="540" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A540">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="541" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A541">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="542" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A542">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="543" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A543">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="544" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A544">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="545" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A545">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="546" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A546">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="547" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A547">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="548" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A548">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="549" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A549">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="550" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A550">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="551" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A551">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="552" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A552">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="553" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A553">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="554" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A554">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="555" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A555">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="556" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A556">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="557" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A557">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="558" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A558">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="559" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A559">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="560" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A560">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="561" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A561">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="562" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A562">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="563" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A563">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="564" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A564">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="565" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A565">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="566" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A566">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="567" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A567">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="568" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A568">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="569" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A569">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="570" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A570">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="571" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A571">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="572" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A572">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="573" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A573">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="574" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A574">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="575" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A575">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="576" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A576">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="577" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A577">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="578" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A578">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="579" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A579">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="580" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A580">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="581" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A581">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="582" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A582">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="583" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A583">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="584" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A584">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="585" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A585">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="586" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A586">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="587" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A587">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="588" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A588">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="589" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A589">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="590" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A590">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="591" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A591">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="592" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A592">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="593" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A593">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="594" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A594">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="595" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A595">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="596" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A596">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="597" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A597">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="598" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A598">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="599" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A599">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="600" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A600">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="601" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A601">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="602" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A602">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="603" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A603">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="604" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A604">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="605" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A605">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="606" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A606">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="607" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A607">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="608" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A608">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="609" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A609">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="610" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A610">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="611" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A611">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="612" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A612">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="613" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A613">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="614" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A614">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="615" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A615">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="616" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A616">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="617" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A617">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="618" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A618">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="619" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A619">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="620" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A620">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="621" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A621">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="622" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A622">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="623" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A623">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="624" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A624">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="625" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A625">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>